<commit_message>
refactor: mapping the tax rate for regions, and regenerate the data with need data
</commit_message>
<xml_diff>
--- a/data/sales_tax_data.xlsx
+++ b/data/sales_tax_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -585,6 +585,126 @@
         <v>2970</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>INV006</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>North</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>2506</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E7" t="n">
+        <v>250.6</v>
+      </c>
+      <c r="F7" t="n">
+        <v>2756.6</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>INV007</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>North</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>1600</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E8" t="n">
+        <v>160</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1760</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>INV008</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>West</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>1800</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="E9" t="n">
+        <v>126</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1926</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>INV009</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>West</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>1900</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="E10" t="n">
+        <v>133</v>
+      </c>
+      <c r="F10" t="n">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>INV0010</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>East</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>2000</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="E11" t="n">
+        <v>180</v>
+      </c>
+      <c r="F11" t="n">
+        <v>2180</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>